<commit_message>
add style to excel
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -75,6 +75,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
   <fills>
     <fill>
@@ -83,8 +104,64 @@
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
   </fills>
   <borders>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -98,6 +175,13 @@
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="3" fillId="4" borderId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="4" fillId="5" borderId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="5" fillId="6" borderId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="6" fillId="7" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="7" fillId="8" borderId="7" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,25 +478,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="7">
         <v>6</v>
       </c>
     </row>

</xml_diff>